<commit_message>
rename first to second
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>sdvfvvfdvd</t>
+  </si>
+  <si>
+    <t>vzfvd</t>
+  </si>
+  <si>
+    <t>vdf</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,7 +125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -323,20 +337,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>